<commit_message>
clarification to seeding sheet
</commit_message>
<xml_diff>
--- a/DCTBFSSeeding.xlsx
+++ b/DCTBFSSeeding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d110c23d71eaefdd/Documents/GitHub/DCTBFightingSimulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23AC14D1-B86B-4059-B0E9-4035EB929E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{23AC14D1-B86B-4059-B0E9-4035EB929E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DEC439D9-9AE4-478F-8FF0-FC9BA140C66D}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="2535" windowWidth="21600" windowHeight="11385" xr2:uid="{E8889201-C7C1-48DA-B9B8-2B3B605CA93E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8889201-C7C1-48DA-B9B8-2B3B605CA93E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
   <si>
     <t>NAME</t>
   </si>
@@ -36,9 +36,6 @@
     <t>TYPE</t>
   </si>
   <si>
-    <t>V/N</t>
-  </si>
-  <si>
     <t>DCTBFightingSimulator Character Seeding and Tournament Match Data</t>
   </si>
   <si>
@@ -178,6 +175,15 @@
   </si>
   <si>
     <t>METAL</t>
+  </si>
+  <si>
+    <t>V/U</t>
+  </si>
+  <si>
+    <t>V = Vanilla</t>
+  </si>
+  <si>
+    <t>U = User-created</t>
   </si>
 </sst>
 </file>
@@ -633,18 +639,19 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -658,39 +665,43 @@
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -700,13 +711,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -716,13 +727,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -732,13 +743,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -748,13 +759,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -764,13 +775,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -780,13 +791,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -796,13 +807,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -812,13 +823,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -828,13 +839,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -844,13 +855,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -860,13 +871,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -876,13 +887,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -892,13 +903,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -908,13 +919,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -924,13 +935,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -940,13 +951,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -956,13 +967,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -972,13 +983,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
@@ -988,13 +999,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
@@ -1004,13 +1015,13 @@
         <v>22</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
@@ -1020,13 +1031,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
@@ -1036,13 +1047,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -1052,13 +1063,13 @@
         <v>25</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
@@ -1068,13 +1079,13 @@
         <v>26</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -1084,13 +1095,13 @@
         <v>27</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
@@ -1100,13 +1111,13 @@
         <v>28</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
@@ -1116,13 +1127,13 @@
         <v>29</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
@@ -1132,13 +1143,13 @@
         <v>30</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>

</xml_diff>

<commit_message>
new seeding, new .exe build
</commit_message>
<xml_diff>
--- a/DCTBFSSeeding.xlsx
+++ b/DCTBFSSeeding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d110c23d71eaefdd/Documents/GitHub/DCTBFightingSimulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{23AC14D1-B86B-4059-B0E9-4035EB929E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6DF9607C-B22E-450E-921C-727D20AFE35E}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{23AC14D1-B86B-4059-B0E9-4035EB929E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E32E5AFB-01F1-451F-9AF9-7276D06E6DFE}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="3915" windowWidth="21600" windowHeight="11385" xr2:uid="{E8889201-C7C1-48DA-B9B8-2B3B605CA93E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="43">
   <si>
     <t>NAME</t>
   </si>
@@ -141,13 +141,19 @@
     <t>Firia</t>
   </si>
   <si>
-    <t>DEP.</t>
-  </si>
-  <si>
     <t>v0.2.0</t>
   </si>
   <si>
     <t>DCTBFightingSimulator Character Seeding and Tournament Match Data (rolling since v0.2.0)</t>
+  </si>
+  <si>
+    <t>v0.2.3</t>
+  </si>
+  <si>
+    <t>DELTA</t>
+  </si>
+  <si>
+    <t>Armaments</t>
   </si>
 </sst>
 </file>
@@ -600,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99F020D-0335-4481-90F9-EE46594DCC6E}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,19 +617,24 @@
     <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -631,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>33</v>
@@ -640,8 +651,20 @@
       <c r="F3" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -656,8 +679,20 @@
       <c r="F4" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -670,8 +705,20 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="5">
+        <v>2</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -684,8 +731,18 @@
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6" s="5">
+        <v>3</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="11"/>
+      <c r="K6" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -698,8 +755,18 @@
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" s="5">
+        <v>4</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -712,8 +779,20 @@
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8" s="5">
+        <v>5</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="11">
+        <v>3</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -726,8 +805,20 @@
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H9" s="5">
+        <v>6</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -740,8 +831,20 @@
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" s="5">
+        <v>7</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="11">
+        <v>2</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -754,8 +857,20 @@
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11" s="5">
+        <v>8</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="11">
+        <v>-2</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -768,8 +883,18 @@
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" s="5">
+        <v>9</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -782,8 +907,20 @@
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13" s="5">
+        <v>10</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>11</v>
       </c>
@@ -796,8 +933,20 @@
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14" s="5">
+        <v>11</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="11">
+        <v>-3</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>12</v>
       </c>
@@ -810,8 +959,18 @@
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H15" s="5">
+        <v>12</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13</v>
       </c>
@@ -824,8 +983,18 @@
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" s="5">
+        <v>13</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>14</v>
       </c>
@@ -838,8 +1007,18 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" s="5">
+        <v>14</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="K17" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>15</v>
       </c>
@@ -852,8 +1031,20 @@
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" s="5">
+        <v>15</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="11">
+        <v>-8</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>16</v>
       </c>
@@ -866,8 +1057,18 @@
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19" s="5">
+        <v>16</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="11"/>
+      <c r="K19" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>17</v>
       </c>
@@ -880,8 +1081,20 @@
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20" s="5">
+        <v>17</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="11">
+        <v>2</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>18</v>
       </c>
@@ -894,8 +1107,20 @@
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21" s="5">
+        <v>18</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="11">
+        <v>-3</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>19</v>
       </c>
@@ -908,8 +1133,18 @@
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22" s="5">
+        <v>19</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>20</v>
       </c>
@@ -922,8 +1157,18 @@
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" s="5">
+        <v>20</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>21</v>
       </c>
@@ -936,8 +1181,18 @@
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24" s="5">
+        <v>21</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="11"/>
+      <c r="K24" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>22</v>
       </c>
@@ -950,8 +1205,18 @@
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H25" s="5">
+        <v>22</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="11"/>
+      <c r="K25" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>23</v>
       </c>
@@ -964,8 +1229,20 @@
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26" s="5">
+        <v>23</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="11">
+        <v>8</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>24</v>
       </c>
@@ -978,8 +1255,18 @@
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H27" s="5">
+        <v>24</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" s="11"/>
+      <c r="K27" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>25</v>
       </c>
@@ -992,8 +1279,20 @@
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28" s="5">
+        <v>25</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="11">
+        <v>-8</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>26</v>
       </c>
@@ -1006,8 +1305,20 @@
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29" s="5">
+        <v>26</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>27</v>
       </c>
@@ -1020,8 +1331,20 @@
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H30" s="5">
+        <v>27</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>28</v>
       </c>
@@ -1034,8 +1357,20 @@
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H31" s="5">
+        <v>28</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" s="11">
+        <v>-10</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>29</v>
       </c>
@@ -1048,8 +1383,20 @@
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H32" s="5">
+        <v>29</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32" s="11">
+        <v>-2</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>30</v>
       </c>
@@ -1062,8 +1409,20 @@
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H33" s="5">
+        <v>30</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J33" s="11">
+        <v>-2</v>
+      </c>
+      <c r="K33" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>31</v>
       </c>
@@ -1074,8 +1433,20 @@
       <c r="D34" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H34" s="5">
+        <v>31</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="11">
+        <v>-2</v>
+      </c>
+      <c r="K34" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>32</v>
       </c>
@@ -1084,6 +1455,32 @@
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" s="5">
+        <v>32</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J35" s="11">
+        <v>-2</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H36" s="5">
+        <v>33</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J36" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K36" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>